<commit_message>
updated simulation setting for toy and low-dimensional settings
</commit_message>
<xml_diff>
--- a/meeting document/Results_06052024_Yu_Ru.xlsx
+++ b/meeting document/Results_06052024_Yu_Ru.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qi/Desktop/Research_at_UW/7_Yu-Ru CV Average vs Aggregate/meeting document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1022481B-B3EC-2E40-8F8F-510C63C6994D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B765AC-3353-604B-A9F9-5123B7B0E71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="2500" windowWidth="27240" windowHeight="16440" activeTab="3" xr2:uid="{C66D189E-0100-5E4E-9B47-E557ACFF23F2}"/>
+    <workbookView xWindow="4040" yWindow="3480" windowWidth="29160" windowHeight="16960" activeTab="3" xr2:uid="{C66D189E-0100-5E4E-9B47-E557ACFF23F2}"/>
   </bookViews>
   <sheets>
     <sheet name="AUC" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Cal intercept" sheetId="3" r:id="rId3"/>
     <sheet name="Cal slope" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -97,7 +97,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -137,8 +137,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E847A819-7A16-354D-ACD5-C5CDD2791865}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView topLeftCell="I1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E0F14F-9C11-4442-9B83-F9824F9BC939}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView topLeftCell="G1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073F4E11-3A8B-FB40-9BCD-BCEABD831569}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:O3"/>
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -969,11 +969,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7019F93D-2C95-0549-855D-0978AA1D42B1}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>